<commit_message>
Ajout des paramètres de vernalization pour les crops
</commit_message>
<xml_diff>
--- a/exampleinputs/crops.xlsx
+++ b/exampleinputs/crops.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="13605"/>
   </bookViews>
   <sheets>
     <sheet name="wheat" sheetId="1" r:id="rId1"/>
     <sheet name="Chickpea" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" iterate="1" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -208,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="170">
   <si>
     <t>CROP:</t>
   </si>
@@ -444,15 +440,6 @@
     <t>durum wheat</t>
   </si>
   <si>
-    <t xml:space="preserve">VernalisationSensitivity </t>
-  </si>
-  <si>
-    <t>PhotoPeriodSensitivity</t>
-  </si>
-  <si>
-    <t>CriticalPhotoPerdiod</t>
-  </si>
-  <si>
     <t>pTbasdev</t>
   </si>
   <si>
@@ -703,6 +690,30 @@
   </si>
   <si>
     <t>list(phenofunction='fThermoCardinal', threshold=100,paramsFunctPheno=list(Tbase=0, Topt1=23, Topt2=27, Tlethal=35))</t>
+  </si>
+  <si>
+    <t>pTbaseVernalization</t>
+  </si>
+  <si>
+    <t>pTopt1Vernalization</t>
+  </si>
+  <si>
+    <t>pTop2Vernalization</t>
+  </si>
+  <si>
+    <t>pTlethalVernalization</t>
+  </si>
+  <si>
+    <t>pVDSAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pVernalisationSensitivity </t>
+  </si>
+  <si>
+    <t>pCriticalPhotoPerdiod</t>
+  </si>
+  <si>
+    <t>pPhotoPeriodSensitivity</t>
   </si>
 </sst>
 </file>
@@ -1326,25 +1337,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64:D71"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="2" customWidth="1"/>
+    <col min="3" max="4" width="11.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -1353,21 +1364,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>77</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
@@ -1381,7 +1392,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
@@ -1395,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
@@ -1409,7 +1420,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>35</v>
       </c>
@@ -1421,7 +1432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>36</v>
       </c>
@@ -1433,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>37</v>
       </c>
@@ -1447,7 +1458,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>38</v>
       </c>
@@ -1461,7 +1472,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>39</v>
       </c>
@@ -1475,7 +1486,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
@@ -1489,7 +1500,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>41</v>
       </c>
@@ -1501,7 +1512,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>42</v>
       </c>
@@ -1515,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>43</v>
       </c>
@@ -1529,7 +1540,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>44</v>
       </c>
@@ -1543,7 +1554,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>45</v>
       </c>
@@ -1557,7 +1568,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>46</v>
       </c>
@@ -1571,7 +1582,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>47</v>
       </c>
@@ -1585,7 +1596,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>48</v>
       </c>
@@ -1597,7 +1608,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>49</v>
       </c>
@@ -1611,7 +1622,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>50</v>
       </c>
@@ -1625,7 +1636,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>51</v>
       </c>
@@ -1639,7 +1650,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>52</v>
       </c>
@@ -1653,7 +1664,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>53</v>
       </c>
@@ -1667,7 +1678,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>54</v>
       </c>
@@ -1681,7 +1692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>55</v>
       </c>
@@ -1695,7 +1706,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>56</v>
       </c>
@@ -1709,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>57</v>
       </c>
@@ -1723,7 +1734,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>58</v>
       </c>
@@ -1737,7 +1748,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>59</v>
       </c>
@@ -1751,7 +1762,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>60</v>
       </c>
@@ -1765,7 +1776,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>61</v>
       </c>
@@ -1779,7 +1790,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>62</v>
       </c>
@@ -1793,7 +1804,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>63</v>
       </c>
@@ -1807,7 +1818,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>64</v>
       </c>
@@ -1819,7 +1830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>65</v>
       </c>
@@ -1833,7 +1844,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>66</v>
       </c>
@@ -1847,7 +1858,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>67</v>
       </c>
@@ -1861,7 +1872,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>68</v>
       </c>
@@ -1873,7 +1884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>69</v>
       </c>
@@ -1887,7 +1898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>70</v>
       </c>
@@ -1901,7 +1912,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>71</v>
       </c>
@@ -1915,7 +1926,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>72</v>
       </c>
@@ -1929,7 +1940,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>73</v>
       </c>
@@ -1943,7 +1954,7 @@
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>74</v>
       </c>
@@ -1957,7 +1968,7 @@
         <v>2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>75</v>
       </c>
@@ -1968,7 +1979,7 @@
         <v>2.0899999999999998E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>76</v>
       </c>
@@ -1982,9 +1993,9 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>6</v>
@@ -1996,9 +2007,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>6</v>
@@ -2010,9 +2021,9 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>6</v>
@@ -2024,9 +2035,9 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>6</v>
@@ -2038,149 +2049,107 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B52" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B57" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="10">
+      <c r="C57" s="10">
         <v>2E-3</v>
       </c>
-      <c r="D52" s="10">
+      <c r="D57" s="10">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="9" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="B58" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="10">
+      <c r="C58" s="10">
         <v>14</v>
       </c>
-      <c r="D53" s="10">
+      <c r="D58" s="10">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" s="9" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C54" s="10">
+      <c r="C59" s="10">
         <v>0.17</v>
       </c>
-      <c r="D54" s="10">
+      <c r="D59" s="10">
         <v>0.17</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="16" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="10">
-        <v>6</v>
-      </c>
-      <c r="D55" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C56" s="10">
-        <v>5</v>
-      </c>
-      <c r="D56" s="10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C57" s="10">
-        <v>8</v>
-      </c>
-      <c r="D57" s="10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C58" s="10">
-        <v>6</v>
-      </c>
-      <c r="D58" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C59" s="10">
-        <v>6</v>
-      </c>
-      <c r="D59" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="17" t="s">
-        <v>29</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C60" s="10">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D60" s="10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C61" s="10">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="D61" s="10">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B62" s="9" t="s">
         <v>24</v>
@@ -2192,124 +2161,189 @@
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="1" customFormat="1">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="10">
+        <v>6</v>
+      </c>
+      <c r="D63" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" s="10">
+        <v>6</v>
+      </c>
+      <c r="D64" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C65" s="10">
+        <v>15</v>
+      </c>
+      <c r="D65" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="10">
+        <v>43</v>
+      </c>
+      <c r="D66" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="10">
+        <v>8</v>
+      </c>
+      <c r="D67" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69"/>
+      <c r="C69" t="s">
+        <v>160</v>
+      </c>
+      <c r="D69" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>88</v>
       </c>
-      <c r="C63" s="30" t="s">
+      <c r="B70"/>
+      <c r="C70" t="s">
+        <v>161</v>
+      </c>
+      <c r="D70" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>89</v>
       </c>
-      <c r="D63" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
+      <c r="B71"/>
+      <c r="C71" t="s">
+        <v>160</v>
+      </c>
+      <c r="D71" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>90</v>
       </c>
-      <c r="B64"/>
-      <c r="C64" t="s">
-        <v>163</v>
-      </c>
-      <c r="D64" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
+      <c r="B72" s="14"/>
+      <c r="C72" t="s">
+        <v>161</v>
+      </c>
+      <c r="D72" t="s">
+        <v>160</v>
+      </c>
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>91</v>
       </c>
-      <c r="B65"/>
-      <c r="C65" t="s">
-        <v>164</v>
-      </c>
-      <c r="D65" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
+      <c r="B73" s="14"/>
+      <c r="C73" t="s">
+        <v>160</v>
+      </c>
+      <c r="D73" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>92</v>
       </c>
-      <c r="B66"/>
-      <c r="C66" t="s">
-        <v>163</v>
-      </c>
-      <c r="D66" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" t="s">
+      <c r="B74" s="14"/>
+      <c r="C74" t="s">
+        <v>161</v>
+      </c>
+      <c r="D74" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>93</v>
       </c>
-      <c r="B67" s="14"/>
-      <c r="C67" t="s">
-        <v>164</v>
-      </c>
-      <c r="D67" t="s">
-        <v>163</v>
-      </c>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5">
-      <c r="A68" t="s">
+      <c r="B75" s="14"/>
+      <c r="C75" t="s">
+        <v>160</v>
+      </c>
+      <c r="D75" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>94</v>
       </c>
-      <c r="B68" s="14"/>
-      <c r="C68" t="s">
-        <v>163</v>
-      </c>
-      <c r="D68" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
-      <c r="A69" t="s">
-        <v>95</v>
-      </c>
-      <c r="B69" s="14"/>
-      <c r="C69" t="s">
-        <v>164</v>
-      </c>
-      <c r="D69" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
-        <v>96</v>
-      </c>
-      <c r="B70" s="14"/>
-      <c r="C70" t="s">
-        <v>163</v>
-      </c>
-      <c r="D70" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>97</v>
-      </c>
-      <c r="B71" s="14"/>
-      <c r="C71" t="s">
-        <v>164</v>
-      </c>
-      <c r="D71" t="s">
-        <v>163</v>
-      </c>
-      <c r="E71" s="2"/>
+      <c r="B76" s="14"/>
+      <c r="C76" t="s">
+        <v>161</v>
+      </c>
+      <c r="D76" t="s">
+        <v>160</v>
+      </c>
+      <c r="E76" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2318,501 +2352,501 @@
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72:C73"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="25">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="25">
         <v>1.61E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="25">
         <v>-5</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="25">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="25">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="25">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="25">
         <v>0.65</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="25">
         <v>1.8</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="25">
         <v>0.8</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="25">
         <v>0.53</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="25">
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="25">
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="25">
         <v>0.13</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="25">
         <v>0.22</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="25">
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="25">
         <v>9999</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="25">
         <v>9999</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="25">
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="25">
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="25">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="25">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="25">
         <v>0.3</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="25">
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B38" s="8"/>
       <c r="C38" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="25">
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="25">
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="25">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="25">
         <v>0.68</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="25">
         <v>1.37E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="25">
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="25">
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="25">
         <v>3.3700000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="25">
         <v>0.45</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="25">
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="27">
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="27">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="27">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="25">
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>23</v>
       </c>
@@ -2821,7 +2855,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
         <v>25</v>
       </c>
@@ -2830,7 +2864,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>26</v>
       </c>
@@ -2839,7 +2873,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>27</v>
       </c>
@@ -2848,7 +2882,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>28</v>
       </c>
@@ -2857,7 +2891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>29</v>
       </c>
@@ -2866,7 +2900,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>30</v>
       </c>
@@ -2875,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>31</v>
       </c>
@@ -2884,110 +2918,105 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B63" s="18"/>
       <c r="C63" s="28">
         <v>8.5</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B64" s="19"/>
       <c r="C64" s="28">
         <v>76.5</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B65" s="20"/>
       <c r="C65" s="29">
         <v>54.5</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B66" s="20"/>
       <c r="C66" s="29">
         <v>76.5</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B67" s="18"/>
       <c r="C67" s="28">
         <v>52.5</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B68" s="18"/>
       <c r="C68" s="28">
         <v>60.1</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B69" s="18"/>
       <c r="C69" s="28">
         <v>54.5</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="29">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C72" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="18" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C73" t="s">
         <v>161</v>
-      </c>
-      <c r="C72" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="C73" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
just update the supporting files following coding of LAI decrease
</commit_message>
<xml_diff>
--- a/exampleinputs/crops.xlsx
+++ b/exampleinputs/crops.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="0" windowWidth="19120" windowHeight="13600" activeTab="2"/>
+    <workbookView xWindow="3120" yWindow="0" windowWidth="24180" windowHeight="13380" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="wheat" sheetId="1" r:id="rId1"/>
     <sheet name="Chickpea" sheetId="2" r:id="rId2"/>
-    <sheet name="allcrops" sheetId="3" r:id="rId3"/>
+    <sheet name="Maize" sheetId="4" r:id="rId3"/>
+    <sheet name="allcrops" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -238,6 +239,112 @@
     <author>Auteur</author>
   </authors>
   <commentList>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Sowing to emergence</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Emergence to end of juvenile</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Silking (last leaf ligule) to physiological maturity (black layer)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A33" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+PLAPOW at density of 8 plants per m2</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Auteur</author>
+  </authors>
+  <commentList>
     <comment ref="A10" authorId="0">
       <text>
         <r>
@@ -358,31 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A104" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>Auteur:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Bioday from sowing to beginning biological nitrogen fixation (in legume crops). This should be set =&gt; bdMAT for non-legume crops. </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A105" authorId="0">
+    <comment ref="A113" authorId="0">
       <text>
         <r>
           <rPr>
@@ -406,12 +489,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="P118" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+this is a procedure (name starting with r because it accsses parameters from ALLDAYDATA (bdEMERJU) and not only the parameters that are passed to all the other photoperiod functions (pp, cpp, ppsen)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="238">
   <si>
     <t>CROP:</t>
   </si>
@@ -986,9 +1093,6 @@
     <t>is.after('booting', 0) &amp; is.before('grainFilling')</t>
   </si>
   <si>
-    <t>is.after('emergence',0) &amp; is.before('grainFilling',0)</t>
-  </si>
-  <si>
     <t>is.after('EMR', 0) &amp; is.before('BOT')</t>
   </si>
   <si>
@@ -1007,19 +1111,127 @@
     <t>bidule</t>
   </si>
   <si>
-    <t>c(SOW=6, EMR=10, EJU=4, TSI=NA,SIL=200,PM=4,MAT=Inf)</t>
-  </si>
-  <si>
     <t>is.after('EJU', 0) &amp; is.before('TSI')</t>
   </si>
   <si>
     <t>is.after('EMR',0) &amp; is.before('SIL')</t>
   </si>
   <si>
-    <t>is.after('EMR', 0) &amp; is.before('SIL', 170)</t>
-  </si>
-  <si>
-    <t>fComputeCoefPhotoperiodMaize</t>
+    <t>temperature_onTU.filter</t>
+  </si>
+  <si>
+    <t>temperature_onBD.filter</t>
+  </si>
+  <si>
+    <t>vernalisation_onTU.filter</t>
+  </si>
+  <si>
+    <t>vernalisation_onBD.filter</t>
+  </si>
+  <si>
+    <t>photoperiod_onTU.filter</t>
+  </si>
+  <si>
+    <t>photoperiod_onBD.filter</t>
+  </si>
+  <si>
+    <t>waterstress_onTU.filter</t>
+  </si>
+  <si>
+    <t>waterstress_onBD.filter</t>
+  </si>
+  <si>
+    <t>is.before('EJU') | is.after('TSI', 0)</t>
+  </si>
+  <si>
+    <t>is.after('leafDevelopment', 0)</t>
+  </si>
+  <si>
+    <t>is.after('EMR', 0)</t>
+  </si>
+  <si>
+    <t>drySoilSurface_onTU.filter</t>
+  </si>
+  <si>
+    <t>text parsed to boolean</t>
+  </si>
+  <si>
+    <t>drySoilSurface_onBD.filter</t>
+  </si>
+  <si>
+    <t>is.before('leafDevelopment')</t>
+  </si>
+  <si>
+    <t>is.after('EMR', 0) &amp; is.before('R7')</t>
+  </si>
+  <si>
+    <t>is.before('EMR')</t>
+  </si>
+  <si>
+    <t>is.after('EMR',0) &amp; is.before('R5')</t>
+  </si>
+  <si>
+    <t>is.after('emergence',0) &amp; is.before('grainFilling')</t>
+  </si>
+  <si>
+    <t>is.after('R3', 2) &amp; is.before('R5', 5.6)</t>
+  </si>
+  <si>
+    <t>is.after('EMR', 0) &amp; is.before('R3', 2)</t>
+  </si>
+  <si>
+    <t>fComputeCoefPhotoperiodLegume</t>
+  </si>
+  <si>
+    <t>actionsAtStageChange</t>
+  </si>
+  <si>
+    <t>c(TSI="rComputeTSISILdurationMaize")</t>
+  </si>
+  <si>
+    <t>Maize</t>
+  </si>
+  <si>
+    <t>B73*MO17 (SC704)</t>
+  </si>
+  <si>
+    <t>bdEMREJU</t>
+  </si>
+  <si>
+    <t>bdSILPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLAPOW8 = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TKILL = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRZLDR = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEC = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GNC = </t>
+  </si>
+  <si>
+    <t>rComputeCoefPhotoperiodMaize</t>
+  </si>
+  <si>
+    <t>is.after('grainFilling', 0)</t>
+  </si>
+  <si>
+    <t>is.after('ANT', 5)</t>
+  </si>
+  <si>
+    <t>LAI_Senescence.filter</t>
+  </si>
+  <si>
+    <t>is.after('R5', 0) &amp; is.before('R7')</t>
+  </si>
+  <si>
+    <t>is.after('R5', 0)</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1241,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1191,8 +1403,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="55"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1277,6 +1515,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="41"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1307,7 +1557,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="104">
+  <cellStyleXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1412,8 +1662,70 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1532,8 +1844,40 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="104">
+  <cellStyles count="166">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
@@ -1585,6 +1929,37 @@
     <cellStyle name="Lien hypertexte" xfId="98" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="100" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="164" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
@@ -1636,6 +2011,37 @@
     <cellStyle name="Lien hypertexte visité" xfId="99" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="101" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="165" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -3005,8 +3411,8 @@
   <sheetPr codeName="Feuil2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72:C79"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3733,23 +4139,696 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P110"/>
+  <dimension ref="A1:C72"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="70">
+        <v>1</v>
+      </c>
+      <c r="B1" s="71">
+        <v>2</v>
+      </c>
+      <c r="C1" s="70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="40" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="72" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="73" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="74" t="s">
+        <v>172</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="67">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="67">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="74" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="67">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="74"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="67"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="74"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="67"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="74"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="67"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="74"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="67"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="74"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="67"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="74"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="67"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="74"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="67"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="74"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="67"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="74" t="s">
+        <v>176</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="68">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="69">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="75"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="68"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="76" t="s">
+        <v>225</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="69">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="76" t="s">
+        <v>226</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="69">
+        <v>33.799999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="76"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="68"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="76"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="68"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="76"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="68"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="76"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="69"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="76"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="68"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="75"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="68"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="75" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="66">
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="75" t="s">
+        <v>227</v>
+      </c>
+      <c r="B33" s="11"/>
+      <c r="C33" s="66">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="66">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="74" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="77" t="s">
+        <v>229</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="68">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="75"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="78"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="66">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="66">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="66">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="75" t="s">
+        <v>140</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="66">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="66">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="75"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="66"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="75" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="66">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="75" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="66">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="66">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="75" t="s">
+        <v>146</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="66">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="75" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" s="66">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="74" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="76" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="68">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="77" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="77" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="68">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="77" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="68">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="75"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="66"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="66">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="75" t="s">
+        <v>155</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" s="66">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" s="66">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="74" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="74" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="66">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C62" s="66">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="74" t="s">
+        <v>161</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="77" t="s">
+        <v>163</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C64" s="68">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="75"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="66"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" s="66">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="66">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="66">
+        <v>1.06E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="66">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="75" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="66">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" s="66">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="75"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="66"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Feuil3" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="P96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P102" sqref="P102"/>
+      <selection pane="bottomRight" activeCell="J110" sqref="J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" customWidth="1"/>
-    <col min="16" max="16" width="45.6640625" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" hidden="1">
@@ -3865,7 +4944,7 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -3896,7 +4975,7 @@
         <v>125</v>
       </c>
       <c r="P6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -3924,6 +5003,9 @@
       <c r="N7" s="10">
         <v>0</v>
       </c>
+      <c r="P7" s="66">
+        <v>38.9</v>
+      </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="8" t="s">
@@ -3950,6 +5032,9 @@
       <c r="N8" s="10">
         <v>0</v>
       </c>
+      <c r="P8" s="66">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="8" t="s">
@@ -3976,6 +5061,9 @@
       <c r="N9" s="10">
         <v>0</v>
       </c>
+      <c r="P9" s="66">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="8" t="s">
@@ -4050,6 +5138,9 @@
       <c r="N12" s="10">
         <v>0</v>
       </c>
+      <c r="P12" s="66">
+        <v>2.1999999999999999E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="8" t="s">
@@ -4076,6 +5167,9 @@
       <c r="N13" s="10">
         <v>0</v>
       </c>
+      <c r="P13" s="66">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="12" t="s">
@@ -4102,6 +5196,9 @@
       <c r="N14" s="10">
         <v>0</v>
       </c>
+      <c r="P14" s="68">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="8" t="s">
@@ -4153,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:16">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="D17" s="10"/>
@@ -4163,7 +5260,7 @@
       <c r="L17" s="10"/>
       <c r="N17" s="10"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:16">
       <c r="A18" s="8" t="s">
         <v>136</v>
       </c>
@@ -4188,8 +5285,11 @@
       <c r="N18" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="P18" s="66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="8" t="s">
         <v>137</v>
       </c>
@@ -4214,8 +5314,11 @@
       <c r="N19" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="P19" s="66">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="8" t="s">
         <v>138</v>
       </c>
@@ -4240,8 +5343,11 @@
       <c r="N20" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="P20" s="66">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="8" t="s">
         <v>139</v>
       </c>
@@ -4266,8 +5372,11 @@
       <c r="N21" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
+      <c r="P21" s="66">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="8" t="s">
         <v>140</v>
       </c>
@@ -4292,8 +5401,11 @@
       <c r="N22" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:14">
+      <c r="P22" s="66">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="8" t="s">
         <v>141</v>
       </c>
@@ -4318,8 +5430,11 @@
       <c r="N23" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:14">
+      <c r="P23" s="66">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="8" t="s">
         <v>142</v>
       </c>
@@ -4343,7 +5458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:16">
       <c r="A25" s="12"/>
       <c r="B25" s="9"/>
       <c r="D25" s="10"/>
@@ -4353,7 +5468,7 @@
       <c r="L25" s="10"/>
       <c r="N25" s="10"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:16">
       <c r="A26" s="8" t="s">
         <v>143</v>
       </c>
@@ -4378,8 +5493,11 @@
       <c r="N26" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:14">
+      <c r="P26" s="66">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="8" t="s">
         <v>144</v>
       </c>
@@ -4404,8 +5522,11 @@
       <c r="N27" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:14">
+      <c r="P27" s="66">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="8" t="s">
         <v>145</v>
       </c>
@@ -4430,8 +5551,11 @@
       <c r="N28" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:14">
+      <c r="P28" s="66">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="8" t="s">
         <v>146</v>
       </c>
@@ -4456,8 +5580,11 @@
       <c r="N29" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:14">
+      <c r="P29" s="66">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="8" t="s">
         <v>147</v>
       </c>
@@ -4482,8 +5609,11 @@
       <c r="N30" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:14">
+      <c r="P30" s="66">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="8" t="s">
         <v>148</v>
       </c>
@@ -4508,8 +5638,11 @@
       <c r="N31" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="P31" s="66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="12" t="s">
         <v>149</v>
       </c>
@@ -4534,8 +5667,11 @@
       <c r="N32" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="P32" s="68">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="12" t="s">
         <v>150</v>
       </c>
@@ -4560,8 +5696,11 @@
       <c r="N33" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="P33" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="12" t="s">
         <v>151</v>
       </c>
@@ -4586,8 +5725,11 @@
       <c r="N34" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="P34" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="12" t="s">
         <v>152</v>
       </c>
@@ -4612,8 +5754,11 @@
       <c r="N35" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="P35" s="68">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="12" t="s">
         <v>153</v>
       </c>
@@ -4638,8 +5783,11 @@
       <c r="N36" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="P36" s="68">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="43"/>
       <c r="B37" s="44"/>
       <c r="C37" s="45"/>
@@ -4651,7 +5799,7 @@
       <c r="L37" s="10"/>
       <c r="N37" s="10"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:16">
       <c r="A38" s="43"/>
       <c r="B38" s="9"/>
       <c r="D38" s="10"/>
@@ -4661,7 +5809,7 @@
       <c r="L38" s="10"/>
       <c r="N38" s="10"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:16">
       <c r="A39" s="43"/>
       <c r="B39" s="9"/>
       <c r="D39" s="10"/>
@@ -4671,7 +5819,7 @@
       <c r="L39" s="10"/>
       <c r="N39" s="10"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:16">
       <c r="A40" s="47"/>
       <c r="B40" s="9"/>
       <c r="D40" s="10"/>
@@ -4681,7 +5829,7 @@
       <c r="L40" s="10"/>
       <c r="N40" s="10"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:16">
       <c r="A41" s="43"/>
       <c r="B41" s="11"/>
       <c r="D41" s="10"/>
@@ -4691,7 +5839,7 @@
       <c r="L41" s="10"/>
       <c r="N41" s="10"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:16">
       <c r="A42" s="43"/>
       <c r="B42" s="9"/>
       <c r="D42" s="10"/>
@@ -4701,7 +5849,7 @@
       <c r="L42" s="10"/>
       <c r="N42" s="10"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:16">
       <c r="A43" s="43"/>
       <c r="B43" s="9"/>
       <c r="D43" s="10"/>
@@ -4711,7 +5859,7 @@
       <c r="L43" s="10"/>
       <c r="N43" s="10"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:16">
       <c r="A44" s="8"/>
       <c r="B44" s="9"/>
       <c r="D44" s="10"/>
@@ -4721,7 +5869,7 @@
       <c r="L44" s="10"/>
       <c r="N44" s="10"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:16">
       <c r="A45" s="8" t="s">
         <v>154</v>
       </c>
@@ -4746,8 +5894,11 @@
       <c r="N45" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="P45" s="66">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" s="8" t="s">
         <v>155</v>
       </c>
@@ -4772,8 +5923,11 @@
       <c r="N46" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="P46" s="66">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" s="8" t="s">
         <v>156</v>
       </c>
@@ -4798,8 +5952,11 @@
       <c r="N47" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:14">
+      <c r="P47" s="66">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" s="13" t="s">
         <v>157</v>
       </c>
@@ -4824,8 +5981,11 @@
       <c r="N48" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:14">
+      <c r="P48" s="66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16">
       <c r="A49" s="13" t="s">
         <v>158</v>
       </c>
@@ -4849,7 +6009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:16">
       <c r="A50" s="8" t="s">
         <v>159</v>
       </c>
@@ -4874,8 +6034,11 @@
       <c r="N50" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:14">
+      <c r="P50" s="66">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
       <c r="A51" s="8" t="s">
         <v>160</v>
       </c>
@@ -4900,8 +6063,11 @@
       <c r="N51" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:14">
+      <c r="P51" s="66">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16">
       <c r="A52" s="8" t="s">
         <v>161</v>
       </c>
@@ -4926,8 +6092,11 @@
       <c r="N52" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:14">
+      <c r="P52" s="66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
       <c r="A53" s="8" t="s">
         <v>162</v>
       </c>
@@ -4951,7 +6120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:16">
       <c r="A54" s="12" t="s">
         <v>163</v>
       </c>
@@ -4976,8 +6145,11 @@
       <c r="N54" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:14">
+      <c r="P54" s="68">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16">
       <c r="A55" s="64"/>
       <c r="B55" s="9"/>
       <c r="D55" s="10"/>
@@ -4987,7 +6159,7 @@
       <c r="L55" s="63"/>
       <c r="N55" s="63"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:16">
       <c r="A56" s="64"/>
       <c r="B56" s="1"/>
       <c r="D56" s="10"/>
@@ -4997,7 +6169,7 @@
       <c r="L56" s="63"/>
       <c r="N56" s="63"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:16">
       <c r="A57" s="64"/>
       <c r="B57" s="1"/>
       <c r="D57" s="10"/>
@@ -5007,7 +6179,7 @@
       <c r="L57" s="63"/>
       <c r="N57" s="63"/>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:16">
       <c r="A58" s="64"/>
       <c r="B58" s="1"/>
       <c r="D58" s="10"/>
@@ -5017,7 +6189,7 @@
       <c r="L58" s="63"/>
       <c r="N58" s="63"/>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:16">
       <c r="A59" s="64"/>
       <c r="B59" s="1"/>
       <c r="D59" s="10"/>
@@ -5027,7 +6199,7 @@
       <c r="L59" s="63"/>
       <c r="N59" s="63"/>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:16">
       <c r="A60" s="47"/>
       <c r="B60" s="9"/>
       <c r="D60" s="15"/>
@@ -5037,7 +6209,7 @@
       <c r="L60" s="15"/>
       <c r="N60" s="15"/>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:16">
       <c r="A61" s="8" t="s">
         <v>164</v>
       </c>
@@ -5062,8 +6234,11 @@
       <c r="N61" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:14">
+      <c r="P61" s="66">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="8" t="s">
         <v>165</v>
       </c>
@@ -5088,8 +6263,11 @@
       <c r="N62" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:14">
+      <c r="P62" s="66">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" s="8" t="s">
         <v>166</v>
       </c>
@@ -5114,8 +6292,11 @@
       <c r="N63" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:14">
+      <c r="P63" s="66">
+        <v>1.06E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16">
       <c r="A64" s="8" t="s">
         <v>167</v>
       </c>
@@ -5140,8 +6321,11 @@
       <c r="N64" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:14">
+      <c r="P64" s="66">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
       <c r="A65" s="8" t="s">
         <v>168</v>
       </c>
@@ -5166,8 +6350,11 @@
       <c r="N65" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:14">
+      <c r="P65" s="66">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" s="8" t="s">
         <v>169</v>
       </c>
@@ -5190,8 +6377,11 @@
       <c r="N66" s="15">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:14">
+      <c r="P66" s="66">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="A67" s="8" t="s">
         <v>170</v>
       </c>
@@ -5217,7 +6407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:16">
       <c r="A68" s="8"/>
       <c r="B68" s="9"/>
       <c r="D68" s="10"/>
@@ -5227,7 +6417,7 @@
       <c r="L68" s="10"/>
       <c r="N68" s="10"/>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:16">
       <c r="A69" s="8" t="s">
         <v>171</v>
       </c>
@@ -5252,8 +6442,11 @@
       <c r="N69" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:14">
+      <c r="P69" s="66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16">
       <c r="A70" s="8" t="s">
         <v>172</v>
       </c>
@@ -5278,8 +6471,11 @@
       <c r="N70" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:14">
+      <c r="P70" s="67">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
       <c r="A71" s="8" t="s">
         <v>173</v>
       </c>
@@ -5304,8 +6500,11 @@
       <c r="N71" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:14">
+      <c r="P71" s="67">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16">
       <c r="A72" s="8" t="s">
         <v>174</v>
       </c>
@@ -5330,8 +6529,11 @@
       <c r="N72" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:14">
+      <c r="P72" s="67">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16">
       <c r="A73" s="50"/>
       <c r="B73" s="9"/>
       <c r="D73" s="48"/>
@@ -5341,7 +6543,7 @@
       <c r="L73" s="48"/>
       <c r="N73" s="48"/>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:16">
       <c r="A74" s="8" t="s">
         <v>175</v>
       </c>
@@ -5367,7 +6569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:16">
       <c r="A75" s="8"/>
       <c r="B75" s="9"/>
       <c r="D75" s="10"/>
@@ -5377,7 +6579,7 @@
       <c r="L75" s="10"/>
       <c r="N75" s="10"/>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:16">
       <c r="A76" s="8" t="s">
         <v>176</v>
       </c>
@@ -5402,8 +6604,11 @@
       <c r="N76" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:14">
+      <c r="P76" s="68">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="8" t="s">
         <v>177</v>
       </c>
@@ -5428,8 +6633,11 @@
       <c r="N77" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:14">
+      <c r="P77" s="69">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16">
       <c r="A78" s="8"/>
       <c r="B78" s="51"/>
       <c r="D78" s="10"/>
@@ -5439,7 +6647,7 @@
       <c r="L78" s="10"/>
       <c r="N78" s="10"/>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:16">
       <c r="A79" s="16" t="s">
         <v>23</v>
       </c>
@@ -5464,8 +6672,11 @@
       <c r="N79" s="10">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:14">
+      <c r="P79" s="68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
       <c r="A80" s="17" t="s">
         <v>25</v>
       </c>
@@ -5489,6 +6700,9 @@
       </c>
       <c r="N80" s="10">
         <v>5</v>
+      </c>
+      <c r="P80" s="69">
+        <v>8.5</v>
       </c>
     </row>
     <row r="81" spans="1:16">
@@ -5515,6 +6729,9 @@
       </c>
       <c r="N81" s="10">
         <v>8</v>
+      </c>
+      <c r="P81" s="69">
+        <v>33.799999999999997</v>
       </c>
     </row>
     <row r="82" spans="1:16">
@@ -5855,29 +7072,34 @@
         <v>24</v>
       </c>
       <c r="D95" s="55">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="F95" s="55">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="H95" s="55">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="J95" s="29">
         <v>12</v>
       </c>
       <c r="L95" s="55">
-        <v>0</v>
+        <v>999</v>
       </c>
       <c r="N95" s="55">
-        <v>0</v>
+        <v>999</v>
+      </c>
+      <c r="P95" s="55">
+        <v>999</v>
       </c>
     </row>
     <row r="96" spans="1:16">
       <c r="A96" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="B96" s="9"/>
+      <c r="B96" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="C96" s="1"/>
       <c r="D96" s="65" t="str">
         <f>"c(germination="&amp;D79&amp;",leafDevelopment="&amp;D80&amp;",tillering="&amp;D81&amp;",stemElongation="&amp;D82&amp;",booting="&amp;D83&amp;",earing="&amp;D84&amp;",anthesis=5,  grainFilling="&amp;D85-5-1.5&amp;", maturation=1.5, senescence="&amp;D86&amp;", harvested=Inf)"</f>
@@ -5895,8 +7117,8 @@
       </c>
       <c r="I96" s="56"/>
       <c r="J96" s="33" t="str">
-        <f>"c(germination="&amp;J79&amp;",leafDevelopment="&amp;J80&amp;",tillering="&amp;J81&amp;",stemElongation="&amp;J82&amp;",booting="&amp;J83&amp;",earing="&amp;J84&amp;",anthesis=5,  grainFilling="&amp;J85-5-1.5&amp;", maturation=1.5, senescence="&amp;J86&amp;", harvested=Inf)"</f>
-        <v>c(germination=8.5,leafDevelopment=36,tillering=5.7,stemElongation=4.3,booting=22,earing=7,anthesis=5,  grainFilling=-6.5, maturation=1.5, senescence=0, harvested=Inf)</v>
+        <f>"c(SOW="&amp;J79&amp;" ,EMR="&amp;J80&amp;", R1="&amp;J81&amp;", R3="&amp;J82&amp;", R5="&amp;J83&amp;", R7="&amp;J84&amp;", R8=Inf)"</f>
+        <v>c(SOW=8.5 ,EMR=36, R1=5.7, R3=4.3, R5=22, R7=7, R8=Inf)</v>
       </c>
       <c r="K96" s="56"/>
       <c r="L96" s="33" t="str">
@@ -5908,408 +7130,692 @@
         <f>"c(SOW="&amp;N79&amp;",EMR="&amp;N80&amp;",TIL="&amp;N81&amp;",SEL="&amp;N82&amp;",BOT="&amp;N83&amp;",EAR="&amp;N84&amp;",ANT="&amp;N85&amp;", PM="&amp;N86&amp;", MAT=Inf)"</f>
         <v>c(SOW=6,EMR=5,TIL=8,SEL=6,BOT=6,EAR=15,ANT=43, PM=8, MAT=Inf)</v>
       </c>
-      <c r="P96" t="s">
-        <v>198</v>
+      <c r="P96" t="str">
+        <f>"c(SOW=" &amp;P79&amp;", EMR="&amp;P80&amp;", EJU=4, TSI=NA, SIL=33.8,PM=4,MAT=Inf)"</f>
+        <v>c(SOW=3, EMR=8.5, EJU=4, TSI=NA, SIL=33.8,PM=4,MAT=Inf)</v>
       </c>
     </row>
     <row r="97" spans="1:16">
-      <c r="A97" s="60" t="s">
-        <v>99</v>
-      </c>
-      <c r="B97" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C97" s="54"/>
+      <c r="A97" s="59" t="s">
+        <v>199</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C97" s="1"/>
       <c r="D97" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E97" s="1"/>
+      <c r="F97" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="G97" s="56"/>
+      <c r="H97" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="I97" s="56"/>
+      <c r="J97" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="K97" s="56"/>
+      <c r="L97" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="M97" s="56"/>
+      <c r="N97" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="P97" s="65" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16">
+      <c r="A98" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C98" s="1"/>
+      <c r="D98" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="E98" s="1"/>
+      <c r="F98" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="G98" s="56"/>
+      <c r="H98" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="I98" s="56"/>
+      <c r="J98" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="K98" s="56"/>
+      <c r="L98" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="M98" s="56"/>
+      <c r="N98" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="P98" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16">
+      <c r="A99" s="60" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C99" s="54"/>
+      <c r="D99" s="65" t="s">
         <v>188</v>
-      </c>
-      <c r="E97" s="14"/>
-      <c r="F97" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="G97" s="57"/>
-      <c r="H97" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="I97" s="57"/>
-      <c r="J97" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="K97" s="57"/>
-      <c r="L97" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="M97" s="57"/>
-      <c r="N97" s="65" t="s">
-        <v>193</v>
-      </c>
-      <c r="P97" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16">
-      <c r="A98" s="61" t="s">
-        <v>100</v>
-      </c>
-      <c r="B98" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C98" s="54"/>
-      <c r="D98" s="65" t="s">
-        <v>188</v>
-      </c>
-      <c r="E98" s="58"/>
-      <c r="F98" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="G98" s="58"/>
-      <c r="H98" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="I98" s="58"/>
-      <c r="J98" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="K98" s="58"/>
-      <c r="L98" s="33" t="s">
-        <v>188</v>
-      </c>
-      <c r="M98" s="58"/>
-      <c r="N98" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="P98" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16">
-      <c r="A99" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D99" s="65" t="s">
-        <v>117</v>
       </c>
       <c r="E99" s="14"/>
       <c r="F99" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="G99" s="14"/>
+        <v>188</v>
+      </c>
+      <c r="G99" s="57"/>
       <c r="H99" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="I99" s="14"/>
+        <v>188</v>
+      </c>
+      <c r="I99" s="57"/>
       <c r="J99" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="K99" s="14"/>
+      <c r="K99" s="57"/>
       <c r="L99" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="M99" s="14"/>
+        <v>188</v>
+      </c>
+      <c r="M99" s="57"/>
       <c r="N99" s="65" t="s">
-        <v>117</v>
+        <v>192</v>
       </c>
       <c r="P99" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:16">
-      <c r="A100" s="59" t="s">
-        <v>102</v>
+      <c r="A100" s="60" t="s">
+        <v>202</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>24</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="C100" s="54"/>
       <c r="D100" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E100" s="14"/>
       <c r="F100" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G100" s="57"/>
       <c r="H100" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I100" s="57"/>
       <c r="J100" s="33" t="s">
-        <v>189</v>
+        <v>117</v>
       </c>
       <c r="K100" s="57"/>
       <c r="L100" s="33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M100" s="57"/>
       <c r="N100" s="65" t="s">
         <v>192</v>
       </c>
       <c r="P100" t="s">
-        <v>200</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:16">
-      <c r="A101" s="59" t="s">
-        <v>103</v>
-      </c>
-      <c r="B101" s="53" t="s">
-        <v>24</v>
+      <c r="A101" s="61" t="s">
+        <v>203</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="C101" s="54"/>
       <c r="D101" s="65" t="s">
-        <v>190</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="E101" s="58"/>
       <c r="F101" s="33" t="s">
-        <v>190</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="G101" s="58"/>
       <c r="H101" s="33" t="s">
-        <v>190</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="I101" s="58"/>
       <c r="J101" s="33" t="s">
-        <v>190</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="K101" s="58"/>
       <c r="L101" s="33" t="s">
-        <v>190</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="M101" s="58"/>
       <c r="N101" s="65" t="s">
-        <v>194</v>
+        <v>117</v>
       </c>
       <c r="P101" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:16">
-      <c r="A102" s="59" t="s">
+      <c r="A102" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C102" s="54"/>
+      <c r="D102" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="E102" s="58"/>
+      <c r="F102" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="G102" s="58"/>
+      <c r="H102" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="I102" s="58"/>
+      <c r="J102" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="K102" s="58"/>
+      <c r="L102" s="33" t="s">
+        <v>188</v>
+      </c>
+      <c r="M102" s="58"/>
+      <c r="N102" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="P102" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16">
+      <c r="A103" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D103" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="E103" s="14"/>
+      <c r="F103" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="G103" s="14"/>
+      <c r="H103" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="I103" s="14"/>
+      <c r="J103" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="K103" s="14"/>
+      <c r="L103" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="M103" s="14"/>
+      <c r="N103" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="P103" t="str">
+        <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;")"</f>
+        <v>is.after('SIL', 6.53846153846154)</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16">
+      <c r="A104" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D104" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="E104" s="14"/>
+      <c r="F104" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="G104" s="14"/>
+      <c r="H104" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="I104" s="14"/>
+      <c r="J104" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="K104" s="14"/>
+      <c r="L104" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="M104" s="14"/>
+      <c r="N104" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="P104" t="str">
+        <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;")"</f>
+        <v>is.after('SIL', 6.53846153846154)</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16">
+      <c r="A105" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D105" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="E105" s="14"/>
+      <c r="F105" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="G105" s="14"/>
+      <c r="H105" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="I105" s="14"/>
+      <c r="J105" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="K105" s="14"/>
+      <c r="L105" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="M105" s="14"/>
+      <c r="N105" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="P105" s="65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16">
+      <c r="A106" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="B106" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D106" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="E106" s="14"/>
+      <c r="F106" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="G106" s="14"/>
+      <c r="H106" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="I106" s="14"/>
+      <c r="J106" s="65" t="s">
+        <v>215</v>
+      </c>
+      <c r="K106" s="14"/>
+      <c r="L106" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="M106" s="14"/>
+      <c r="N106" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="P106" s="65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16">
+      <c r="A107" s="59" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D107" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="E107" s="14"/>
+      <c r="F107" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="G107" s="57"/>
+      <c r="H107" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="I107" s="57"/>
+      <c r="J107" s="33" t="s">
+        <v>219</v>
+      </c>
+      <c r="K107" s="57"/>
+      <c r="L107" s="33" t="s">
+        <v>189</v>
+      </c>
+      <c r="M107" s="57"/>
+      <c r="N107" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="P107" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16">
+      <c r="A108" s="59" t="s">
+        <v>103</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C108" s="54"/>
+      <c r="D108" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="F108" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="H108" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="J108" s="33" t="s">
+        <v>218</v>
+      </c>
+      <c r="L108" s="33" t="s">
+        <v>190</v>
+      </c>
+      <c r="N108" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="P108" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16">
+      <c r="A109" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C109" s="54"/>
+      <c r="D109" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="F109" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="H109" s="65" t="s">
+        <v>233</v>
+      </c>
+      <c r="J109" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="L109" s="79" t="s">
+        <v>233</v>
+      </c>
+      <c r="N109" s="65" t="s">
+        <v>234</v>
+      </c>
+      <c r="P109" t="str">
+        <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;")"</f>
+        <v>is.after('SIL', 6.53846153846154)</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16">
+      <c r="A110" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="B102" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C102" s="54"/>
-      <c r="D102" s="65" t="str">
+      <c r="B110" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C110" s="54"/>
+      <c r="D110" s="65" t="str">
         <f>"is.after('grainFilling', 0) &amp; is.before('maturation')"</f>
         <v>is.after('grainFilling', 0) &amp; is.before('maturation')</v>
       </c>
-      <c r="F102" s="33" t="str">
+      <c r="F110" s="33" t="str">
         <f>"is.after('grainFilling', 0) &amp; is.before('maturation')"</f>
         <v>is.after('grainFilling', 0) &amp; is.before('maturation')</v>
       </c>
-      <c r="H102" s="33" t="str">
+      <c r="H110" s="33" t="str">
         <f>"is.after('grainFilling', 0) &amp; is.before('maturation')"</f>
         <v>is.after('grainFilling', 0) &amp; is.before('maturation')</v>
       </c>
-      <c r="J102" s="33" t="str">
+      <c r="J110" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="L110" s="33" t="str">
         <f>"is.after('grainFilling', 0) &amp; is.before('maturation')"</f>
         <v>is.after('grainFilling', 0) &amp; is.before('maturation')</v>
       </c>
-      <c r="L102" s="33" t="str">
-        <f>"is.after('grainFilling', 0) &amp; is.before('maturation')"</f>
-        <v>is.after('grainFilling', 0) &amp; is.before('maturation')</v>
-      </c>
-      <c r="N102" s="65" t="str">
+      <c r="N110" s="65" t="str">
         <f>"is.after('ANT', 5) &amp; is.before('ANT', "&amp; N85-1.5 &amp; ")"</f>
         <v>is.after('ANT', 5) &amp; is.before('ANT', 41.5)</v>
       </c>
-      <c r="P102" t="str">
-        <f>"is.after('SIL', 170) &amp; is.before('SIL', "&amp; 0.95*250&amp;")"</f>
-        <v>is.after('SIL', 170) &amp; is.before('SIL', 237.5)</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16">
-      <c r="A103" s="61" t="s">
+      <c r="P110" t="str">
+        <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;") &amp; is.before('SIL', "&amp; 0.95*P81&amp;")"</f>
+        <v>is.after('SIL', 6.53846153846154) &amp; is.before('SIL', 32.11)</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16">
+      <c r="A111" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B103" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C103" s="54"/>
-      <c r="D103" s="65" t="s">
+      <c r="B111" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="C111" s="54"/>
+      <c r="D111" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="F103" s="33" t="s">
+      <c r="F111" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="H103" s="33" t="s">
+      <c r="H111" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="J103" s="33" t="s">
+      <c r="J111" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="L103" s="33" t="s">
+      <c r="L111" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="N103" s="65" t="s">
+      <c r="N111" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="P103" t="s">
+      <c r="P111" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
-      <c r="A104" s="62" t="s">
+    <row r="112" spans="1:16">
+      <c r="A112" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="B104" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D104" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="F104" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="H104" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="J104" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="L104" s="33" t="s">
-        <v>191</v>
-      </c>
-      <c r="N104" s="65" t="s">
-        <v>195</v>
-      </c>
-      <c r="P104" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16">
-      <c r="A105" s="64" t="s">
+      <c r="B112" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D112" s="65" t="s">
+        <v>217</v>
+      </c>
+      <c r="F112" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="H112" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="J112" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="L112" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="N112" s="65" t="s">
+        <v>194</v>
+      </c>
+      <c r="P112" t="str">
+        <f>"is.after('EMR', 0) &amp; is.before('SIL', "&amp;170/(P70-P69)&amp;")"</f>
+        <v>is.after('EMR', 0) &amp; is.before('SIL', 6.53846153846154)</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16">
+      <c r="A113" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="B105" s="9"/>
-      <c r="D105" s="10">
+      <c r="B113" s="9"/>
+      <c r="D113" s="10">
         <v>-1</v>
       </c>
-      <c r="F105" s="63">
+      <c r="F113" s="63">
         <v>-1</v>
       </c>
-      <c r="H105" s="63">
+      <c r="H113" s="63">
         <v>-1</v>
       </c>
-      <c r="J105" s="25"/>
-      <c r="L105" s="63">
+      <c r="J113" s="25"/>
+      <c r="L113" s="63">
         <v>-1</v>
       </c>
-      <c r="N105" s="63">
+      <c r="N113" s="63">
         <v>-1</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
-      <c r="A106" s="64" t="s">
+    <row r="114" spans="1:16">
+      <c r="A114" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="B106" s="1"/>
-      <c r="D106" s="10">
-        <v>0</v>
-      </c>
-      <c r="F106" s="63">
-        <v>0</v>
-      </c>
-      <c r="H106" s="63">
-        <v>0</v>
-      </c>
-      <c r="J106" s="25"/>
-      <c r="L106" s="63">
-        <v>0</v>
-      </c>
-      <c r="N106" s="63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16">
-      <c r="A107" s="64" t="s">
+      <c r="B114" s="1"/>
+      <c r="D114" s="10">
+        <v>0</v>
+      </c>
+      <c r="F114" s="63">
+        <v>0</v>
+      </c>
+      <c r="H114" s="63">
+        <v>0</v>
+      </c>
+      <c r="J114" s="25"/>
+      <c r="L114" s="63">
+        <v>0</v>
+      </c>
+      <c r="N114" s="63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16">
+      <c r="A115" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="B107" s="1"/>
-      <c r="D107" s="10">
+      <c r="B115" s="1"/>
+      <c r="D115" s="10">
         <v>8</v>
       </c>
-      <c r="F107" s="63">
+      <c r="F115" s="63">
         <v>8</v>
       </c>
-      <c r="H107" s="63">
+      <c r="H115" s="63">
         <v>8</v>
       </c>
-      <c r="J107" s="25"/>
-      <c r="L107" s="63">
+      <c r="J115" s="25"/>
+      <c r="L115" s="63">
         <v>8</v>
       </c>
-      <c r="N107" s="63">
+      <c r="N115" s="63">
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
-      <c r="A108" s="64" t="s">
+    <row r="116" spans="1:16">
+      <c r="A116" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="B108" s="1"/>
-      <c r="D108" s="10">
+      <c r="B116" s="1"/>
+      <c r="D116" s="10">
         <v>12</v>
       </c>
-      <c r="F108" s="63">
+      <c r="F116" s="63">
         <v>12</v>
       </c>
-      <c r="H108" s="63">
+      <c r="H116" s="63">
         <v>12</v>
       </c>
-      <c r="J108" s="25"/>
-      <c r="L108" s="63">
+      <c r="J116" s="25"/>
+      <c r="L116" s="63">
         <v>12</v>
       </c>
-      <c r="N108" s="63">
+      <c r="N116" s="63">
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
-      <c r="A109" s="64" t="s">
+    <row r="117" spans="1:16">
+      <c r="A117" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="B109" s="1"/>
-      <c r="D109" s="10">
+      <c r="B117" s="1"/>
+      <c r="D117" s="10">
         <v>50</v>
       </c>
-      <c r="F109" s="63">
+      <c r="F117" s="63">
         <v>50</v>
       </c>
-      <c r="H109" s="63">
+      <c r="H117" s="63">
         <v>50</v>
       </c>
-      <c r="J109" s="25"/>
-      <c r="L109" s="63">
+      <c r="J117" s="25"/>
+      <c r="L117" s="63">
         <v>50</v>
       </c>
-      <c r="N109" s="63">
+      <c r="N117" s="63">
         <v>50</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
-      <c r="A110" t="s">
+    <row r="118" spans="1:16">
+      <c r="A118" t="s">
         <v>186</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D118" t="s">
         <v>187</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F118" t="s">
         <v>187</v>
       </c>
-      <c r="H110" t="s">
+      <c r="H118" t="s">
         <v>187</v>
       </c>
-      <c r="J110" t="s">
+      <c r="J118" t="s">
+        <v>220</v>
+      </c>
+      <c r="L118" t="s">
         <v>187</v>
       </c>
-      <c r="L110" t="s">
+      <c r="N118" t="s">
         <v>187</v>
       </c>
-      <c r="N110" t="s">
-        <v>187</v>
-      </c>
-      <c r="P110" t="s">
-        <v>202</v>
+      <c r="P118" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="119" spans="1:16">
+      <c r="A119" s="64" t="s">
+        <v>221</v>
+      </c>
+      <c r="P119" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update crop parameters for change in variable names
</commit_message>
<xml_diff>
--- a/exampleinputs/crops.xlsx
+++ b/exampleinputs/crops.xlsx
@@ -518,7 +518,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="239">
   <si>
     <t>CROP:</t>
   </si>
@@ -1168,9 +1168,6 @@
     <t>is.before('EMR')</t>
   </si>
   <si>
-    <t>is.after('EMR',0) &amp; is.before('R5')</t>
-  </si>
-  <si>
     <t>is.after('emergence',0) &amp; is.before('grainFilling')</t>
   </si>
   <si>
@@ -1232,6 +1229,12 @@
   </si>
   <si>
     <t>is.after('R5', 0)</t>
+  </si>
+  <si>
+    <t>is.after('EMR',0) &amp; is.before('R7')</t>
+  </si>
+  <si>
+    <t>is.after('leafDevelopment',0) &amp; is.before('maturation')</t>
   </si>
 </sst>
 </file>
@@ -1557,11 +1560,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="166">
+  <cellStyleXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1877,7 +1884,7 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="166">
+  <cellStyles count="170">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="6" builtinId="8" hidden="1"/>
@@ -1960,6 +1967,8 @@
     <cellStyle name="Lien hypertexte" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="162" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="168" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9" hidden="1"/>
@@ -2042,6 +2051,8 @@
     <cellStyle name="Lien hypertexte visité" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="163" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="169" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -4179,7 +4190,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="72" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -4188,7 +4199,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="73" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -4315,7 +4326,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="76" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>17</v>
@@ -4326,7 +4337,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="76" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>17</v>
@@ -4389,7 +4400,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="66">
@@ -4409,7 +4420,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="74" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>6</v>
@@ -4420,7 +4431,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="77" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>7</v>
@@ -4666,7 +4677,7 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="74" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B60" s="9" t="s">
         <v>16</v>
@@ -4770,7 +4781,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>20</v>
@@ -4812,11 +4823,11 @@
   <dimension ref="A1:P119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="F96" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J110" sqref="J110"/>
+      <selection pane="bottomRight" activeCell="J111" sqref="J111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -4828,6 +4839,7 @@
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.1640625" customWidth="1"/>
     <col min="14" max="14" width="11.6640625" customWidth="1"/>
+    <col min="15" max="15" width="36.6640625" customWidth="1"/>
     <col min="16" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7503,7 +7515,7 @@
       </c>
       <c r="I107" s="57"/>
       <c r="J107" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="K107" s="57"/>
       <c r="L107" s="33" t="s">
@@ -7535,7 +7547,7 @@
         <v>190</v>
       </c>
       <c r="J108" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L108" s="33" t="s">
         <v>190</v>
@@ -7549,29 +7561,29 @@
     </row>
     <row r="109" spans="1:16">
       <c r="A109" s="59" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>211</v>
       </c>
       <c r="C109" s="54"/>
       <c r="D109" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="F109" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="H109" s="65" t="s">
+        <v>232</v>
+      </c>
+      <c r="J109" s="33" t="s">
+        <v>236</v>
+      </c>
+      <c r="L109" s="79" t="s">
+        <v>232</v>
+      </c>
+      <c r="N109" s="65" t="s">
         <v>233</v>
-      </c>
-      <c r="F109" s="65" t="s">
-        <v>233</v>
-      </c>
-      <c r="H109" s="65" t="s">
-        <v>233</v>
-      </c>
-      <c r="J109" s="33" t="s">
-        <v>237</v>
-      </c>
-      <c r="L109" s="79" t="s">
-        <v>233</v>
-      </c>
-      <c r="N109" s="65" t="s">
-        <v>234</v>
       </c>
       <c r="P109" t="str">
         <f>"is.after('SIL', "&amp;170/(P70-P69)&amp;")"</f>
@@ -7599,7 +7611,7 @@
         <v>is.after('grainFilling', 0) &amp; is.before('maturation')</v>
       </c>
       <c r="J110" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L110" s="33" t="str">
         <f>"is.after('grainFilling', 0) &amp; is.before('maturation')"</f>
@@ -7623,25 +7635,27 @@
       </c>
       <c r="C111" s="54"/>
       <c r="D111" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="F111" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="H111" s="33" t="s">
-        <v>117</v>
+        <v>238</v>
+      </c>
+      <c r="F111" s="65" t="s">
+        <v>238</v>
+      </c>
+      <c r="H111" s="65" t="s">
+        <v>238</v>
       </c>
       <c r="J111" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="L111" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="N111" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="P111" t="s">
-        <v>117</v>
+        <v>214</v>
+      </c>
+      <c r="L111" s="65" t="s">
+        <v>238</v>
+      </c>
+      <c r="N111" s="65" t="str">
+        <f>"is.after('EMR',  0) &amp; is.before('ANT', "&amp; N85-1.5 &amp; ")"</f>
+        <v>is.after('EMR',  0) &amp; is.before('ANT', 41.5)</v>
+      </c>
+      <c r="P111" t="str">
+        <f>"is.after('EMR',0) &amp; is.before('SIL', "&amp; 0.95*P81&amp;")"</f>
+        <v>is.after('EMR',0) &amp; is.before('SIL', 32.11)</v>
       </c>
     </row>
     <row r="112" spans="1:16">
@@ -7652,19 +7666,19 @@
         <v>211</v>
       </c>
       <c r="D112" s="65" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F112" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="H112" s="33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J112" s="33" t="s">
+        <v>237</v>
+      </c>
+      <c r="L112" s="33" t="s">
         <v>216</v>
-      </c>
-      <c r="L112" s="33" t="s">
-        <v>217</v>
       </c>
       <c r="N112" s="65" t="s">
         <v>194</v>
@@ -7798,7 +7812,7 @@
         <v>187</v>
       </c>
       <c r="J118" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L118" t="s">
         <v>187</v>
@@ -7807,15 +7821,15 @@
         <v>187</v>
       </c>
       <c r="P118" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:16">
       <c r="A119" s="64" t="s">
+        <v>220</v>
+      </c>
+      <c r="P119" t="s">
         <v>221</v>
-      </c>
-      <c r="P119" t="s">
-        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>